<commit_message>
End of class Feb-03
</commit_message>
<xml_diff>
--- a/Spring 2023 FRIDAYS roster Scripting.xlsx
+++ b/Spring 2023 FRIDAYS roster Scripting.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fscj-my.sharepoint.com/personal/pamela_brauda_fscj_edu/Documents/WorkingConnections/FF-FebruaryMarch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbrauda\Documents\2023SpringNetworkScripting5Fridays\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{0E9D4F06-1B5B-4A3D-BC91-EA7E515BB24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17265F4F-E8F8-4AE7-AA43-073117DA9EB2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B93CCAB-DD6D-4203-8545-7163DE457B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="1470" windowWidth="17130" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="1035" windowWidth="21345" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rosters" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Rosters!$A$1:$M$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Rosters!$A$1:$M$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t>Morning</t>
   </si>
@@ -113,18 +113,6 @@
   </si>
   <si>
     <t>Cabrillo College</t>
-  </si>
-  <si>
-    <t>Matt</t>
-  </si>
-  <si>
-    <t>Klint</t>
-  </si>
-  <si>
-    <t>klintm@clarkstate.edu</t>
-  </si>
-  <si>
-    <t>Clark State College</t>
   </si>
   <si>
     <t>Yaritza</t>
@@ -840,11 +828,11 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -852,11 +840,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1221,10 +1209,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A15" sqref="A15:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,37 +1225,37 @@
   <sheetData>
     <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C1" s="12"/>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="14"/>
+      <c r="F1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="14"/>
+      <c r="H1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="14"/>
+      <c r="J1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="14"/>
+      <c r="L1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="18"/>
+      <c r="M1" s="14"/>
     </row>
     <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
@@ -1305,10 +1293,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="2"/>
@@ -1323,10 +1311,10 @@
     </row>
     <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="2"/>
@@ -1344,12 +1332,12 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="13"/>
+        <v>39</v>
+      </c>
+      <c r="D5" s="17"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -1362,12 +1350,12 @@
     </row>
     <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="14"/>
+        <v>41</v>
+      </c>
+      <c r="D6" s="18"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1388,7 +1376,7 @@
       <c r="C7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="13"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -1406,7 +1394,7 @@
       <c r="C8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="14"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1422,12 +1410,12 @@
         <v>4</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="13"/>
+        <v>31</v>
+      </c>
+      <c r="D9" s="17"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -1440,12 +1428,12 @@
     </row>
     <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="D10" s="18"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -1466,7 +1454,7 @@
       <c r="C11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="13"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -1484,7 +1472,7 @@
       <c r="C12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="14"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -1505,7 +1493,7 @@
       <c r="C13" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="13"/>
+      <c r="D13" s="17"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -1523,7 +1511,7 @@
       <c r="C14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="14"/>
+      <c r="D14" s="18"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -1536,15 +1524,15 @@
     </row>
     <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="13"/>
+        <v>20</v>
+      </c>
+      <c r="D15" s="17"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -1557,12 +1545,12 @@
     </row>
     <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="D16" s="18"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -1575,15 +1563,15 @@
     </row>
     <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="13"/>
+        <v>43</v>
+      </c>
+      <c r="D17" s="17"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1596,12 +1584,12 @@
     </row>
     <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="D18" s="18"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -1614,15 +1602,15 @@
     </row>
     <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="13"/>
+        <v>27</v>
+      </c>
+      <c r="D19" s="17"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1635,12 +1623,12 @@
     </row>
     <row r="20" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="14"/>
+        <v>29</v>
+      </c>
+      <c r="D20" s="18"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
@@ -1653,15 +1641,15 @@
     </row>
     <row r="21" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="13"/>
+        <v>50</v>
+      </c>
+      <c r="D21" s="17"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -1673,13 +1661,13 @@
       <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>28</v>
+      <c r="B22" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="D22" s="18"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -1692,15 +1680,15 @@
     </row>
     <row r="23" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="13"/>
+        <v>16</v>
+      </c>
+      <c r="D23" s="4"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -1712,13 +1700,13 @@
       <c r="M23" s="5"/>
     </row>
     <row r="24" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
-        <v>55</v>
+      <c r="B24" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="14"/>
+        <v>18</v>
+      </c>
+      <c r="D24" s="4"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -1731,13 +1719,13 @@
     </row>
     <row r="25" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
@@ -1752,10 +1740,10 @@
     </row>
     <row r="26" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
@@ -1770,13 +1758,13 @@
     </row>
     <row r="27" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="5"/>
@@ -1790,83 +1778,43 @@
       <c r="M27" s="5"/>
     </row>
     <row r="28" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
-        <v>40</v>
+      <c r="B28" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="D28" s="4"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-    </row>
-    <row r="29" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>15</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-    </row>
-    <row r="30" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C29">
-    <sortCondition ref="C3:C29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C27">
+    <sortCondition ref="C3:C27"/>
   </sortState>
-  <mergeCells count="16">
+  <mergeCells count="15">
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="72" orientation="landscape" r:id="rId1"/>

</xml_diff>